<commit_message>
[CLUB 287] Update home member and personal config
</commit_message>
<xml_diff>
--- a/public/excels/member_create_template.xlsx
+++ b/public/excels/member_create_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55865A7B-5780-4DF6-9EDC-243A7BC4D991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B69297A-5326-4C68-AA21-A67A7439E876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{53A5229A-B26F-4CE3-9CC4-B2B53A3926C8}"/>
+    <workbookView xWindow="14235" yWindow="1560" windowWidth="21150" windowHeight="12510" xr2:uid="{53A5229A-B26F-4CE3-9CC4-B2B53A3926C8}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Họ</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>YYYY-MM-dd</t>
+  </si>
+  <si>
+    <t>K18411C</t>
   </si>
   <si>
     <t>Ví dụ</t>
@@ -400,14 +403,32 @@
     </r>
   </si>
   <si>
-    <t>Bạn KHÔNG nên thay đổi vị trị/thứ tự các cột</t>
+    <t>K184111445</t>
+  </si>
+  <si>
+    <t>Địa chỉ rất dài dài dài dài dài dài và cần xem xét</t>
+  </si>
+  <si>
+    <t>0901498235</t>
+  </si>
+  <si>
+    <t>Nam Định</t>
+  </si>
+  <si>
+    <t>Quang Huế</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>vuquanghuy2k10@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +495,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -513,10 +542,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -532,8 +562,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -846,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1229243D-F897-4B52-B4C5-6D73D6080D52}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,56 +935,55 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{0CBC94AA-33BE-4846-836C-532F034D7F62}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007CAB78-C8E1-4C45-9605-2C0FF307B7DA}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +996,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -979,199 +1010,194 @@
         <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>